<commit_message>
excelTool.py now can read in data
</commit_message>
<xml_diff>
--- a/rsc/champs.xlsx
+++ b/rsc/champs.xlsx
@@ -20,7 +20,16 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="121">
+  <si>
+    <t xml:space="preserve">champs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">attributes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cost</t>
+  </si>
   <si>
     <t xml:space="preserve">Aatrox</t>
   </si>
@@ -580,10 +589,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C60"/>
+  <dimension ref="A1:C61"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E62" activeCellId="0" sqref="E62"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -599,656 +608,667 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="n">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="0" t="n">
-        <v>1</v>
+        <v>4</v>
+      </c>
+      <c r="C2" s="1" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="0" t="n">
-        <v>3</v>
+        <v>6</v>
+      </c>
+      <c r="C3" s="1" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="C4" s="1" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="0" t="n">
-        <v>4</v>
+        <v>10</v>
+      </c>
+      <c r="C5" s="1" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="0" t="n">
-        <v>3</v>
+        <v>12</v>
+      </c>
+      <c r="C6" s="1" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" s="0" t="n">
-        <v>4</v>
+        <v>14</v>
+      </c>
+      <c r="C7" s="1" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8" s="0" t="n">
-        <v>5</v>
+        <v>16</v>
+      </c>
+      <c r="C8" s="1" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9" s="0" t="n">
-        <v>3</v>
+        <v>18</v>
+      </c>
+      <c r="C9" s="1" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C10" s="0" t="n">
-        <v>1</v>
+        <v>20</v>
+      </c>
+      <c r="C10" s="1" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C11" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="C11" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C12" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="C12" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C13" s="0" t="n">
-        <v>3</v>
+        <v>26</v>
+      </c>
+      <c r="C13" s="1" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C14" s="0" t="n">
-        <v>4</v>
+        <v>28</v>
+      </c>
+      <c r="C14" s="1" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C15" s="0" t="n">
-        <v>1</v>
+        <v>30</v>
+      </c>
+      <c r="C15" s="1" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C16" s="0" t="n">
-        <v>2</v>
+        <v>32</v>
+      </c>
+      <c r="C16" s="1" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C17" s="0" t="n">
-        <v>5</v>
+        <v>34</v>
+      </c>
+      <c r="C17" s="1" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C18" s="0" t="n">
-        <v>3</v>
+        <v>36</v>
+      </c>
+      <c r="C18" s="1" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C19" s="0" t="n">
-        <v>5</v>
+        <v>38</v>
+      </c>
+      <c r="C19" s="1" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C20" s="0" t="n">
-        <v>2</v>
+        <v>40</v>
+      </c>
+      <c r="C20" s="1" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C21" s="0" t="n">
-        <v>1</v>
+        <v>42</v>
+      </c>
+      <c r="C21" s="1" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C22" s="0" t="n">
-        <v>4</v>
+        <v>44</v>
+      </c>
+      <c r="C22" s="1" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C23" s="0" t="n">
+        <v>46</v>
+      </c>
+      <c r="C23" s="1" t="n">
         <v>4</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C24" s="0" t="n">
-        <v>1</v>
+        <v>48</v>
+      </c>
+      <c r="C24" s="1" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C25" s="0" t="n">
-        <v>2</v>
+        <v>50</v>
+      </c>
+      <c r="C25" s="1" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="C26" s="0" t="n">
-        <v>1</v>
+        <v>52</v>
+      </c>
+      <c r="C26" s="1" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C27" s="0" t="n">
+        <v>54</v>
+      </c>
+      <c r="C27" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="C28" s="0" t="n">
-        <v>4</v>
+        <v>56</v>
+      </c>
+      <c r="C28" s="1" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="C29" s="0" t="n">
+        <v>58</v>
+      </c>
+      <c r="C29" s="1" t="n">
         <v>4</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="C30" s="0" t="n">
-        <v>5</v>
+        <v>60</v>
+      </c>
+      <c r="C30" s="1" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="C31" s="0" t="n">
-        <v>2</v>
+        <v>62</v>
+      </c>
+      <c r="C31" s="1" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="C32" s="0" t="n">
-        <v>1</v>
+      <c r="C32" s="1" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C33" s="0" t="n">
-        <v>4</v>
+        <v>65</v>
+      </c>
+      <c r="C33" s="1" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="C34" s="0" t="n">
+        <v>67</v>
+      </c>
+      <c r="C34" s="1" t="n">
         <v>4</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="C35" s="0" t="n">
-        <v>2</v>
+        <v>69</v>
+      </c>
+      <c r="C35" s="1" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C36" s="0" t="n">
-        <v>4</v>
+        <v>71</v>
+      </c>
+      <c r="C36" s="1" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="C37" s="0" t="n">
-        <v>2</v>
+        <v>73</v>
+      </c>
+      <c r="C37" s="1" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="C38" s="0" t="n">
-        <v>5</v>
+        <v>75</v>
+      </c>
+      <c r="C38" s="1" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="C39" s="0" t="n">
-        <v>1</v>
+        <v>77</v>
+      </c>
+      <c r="C39" s="1" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="C40" s="0" t="n">
-        <v>2</v>
+        <v>79</v>
+      </c>
+      <c r="C40" s="1" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="C41" s="0" t="n">
+        <v>81</v>
+      </c>
+      <c r="C41" s="1" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C42" s="0" t="n">
-        <v>5</v>
+        <v>83</v>
+      </c>
+      <c r="C42" s="1" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="C43" s="0" t="n">
-        <v>2</v>
+        <v>85</v>
+      </c>
+      <c r="C43" s="1" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="C44" s="0" t="n">
-        <v>1</v>
+        <v>87</v>
+      </c>
+      <c r="C44" s="1" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="C45" s="0" t="n">
-        <v>3</v>
+        <v>89</v>
+      </c>
+      <c r="C45" s="1" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="C46" s="0" t="n">
-        <v>4</v>
+        <v>91</v>
+      </c>
+      <c r="C46" s="1" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C47" s="0" t="n">
+        <v>93</v>
+      </c>
+      <c r="C47" s="1" t="n">
         <v>4</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="C48" s="0" t="n">
-        <v>3</v>
+        <v>6</v>
+      </c>
+      <c r="C48" s="1" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="C49" s="0" t="n">
-        <v>2</v>
+        <v>96</v>
+      </c>
+      <c r="C49" s="1" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="C50" s="0" t="n">
-        <v>3</v>
+        <v>98</v>
+      </c>
+      <c r="C50" s="1" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="C51" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="C51" s="1" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="C52" s="0" t="n">
-        <v>5</v>
+        <v>102</v>
+      </c>
+      <c r="C52" s="1" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="C53" s="0" t="n">
-        <v>3</v>
+        <v>104</v>
+      </c>
+      <c r="C53" s="1" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="C54" s="0" t="n">
-        <v>5</v>
+        <v>106</v>
+      </c>
+      <c r="C54" s="1" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="C55" s="0" t="n">
+        <v>108</v>
+      </c>
+      <c r="C55" s="1" t="n">
         <v>5</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="1" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="C56" s="0" t="n">
-        <v>1</v>
+        <v>110</v>
+      </c>
+      <c r="C56" s="1" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="C57" s="0" t="n">
-        <v>3</v>
+        <v>112</v>
+      </c>
+      <c r="C57" s="1" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="C58" s="0" t="n">
-        <v>2</v>
+        <v>114</v>
+      </c>
+      <c r="C58" s="1" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="C59" s="0" t="n">
-        <v>3</v>
+        <v>116</v>
+      </c>
+      <c r="C59" s="1" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="C60" s="0" t="n">
+        <v>118</v>
+      </c>
+      <c r="C60" s="1" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C61" s="1" t="n">
         <v>2</v>
       </c>
     </row>

</xml_diff>